<commit_message>
Added info on numbering of the feet skin triangles in skinGui ini generators.
</commit_message>
<xml_diff>
--- a/app/skinGui/iniGenerators/left_foot_ini_generator.xlsx
+++ b/app/skinGui/iniGenerators/left_foot_ini_generator.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\icub-main\app\skinGui\iniGenerators\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="12570" yWindow="-270" windowWidth="12600" windowHeight="12975" activeTab="1"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="bottom" sheetId="2" r:id="rId2"/>
     <sheet name="final ini" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -117,7 +122,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -825,6 +830,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -2025,6 +2033,810 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:endParaRPr lang="it-IT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>212912</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>280148</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect l="18111" r="7694"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3473824" y="6477000"/>
+          <a:ext cx="7115736" cy="3971429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>560295</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>895788</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>1363</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9031942" y="7182971"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>0</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>40342</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>375835</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>19292</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8511989" y="7581900"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>271183</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>147917</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>606676</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>14809</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7879977" y="7386917"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>748554</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>42582</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>120341</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>99974</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7393642" y="7853082"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>878542</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>94130</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>250329</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>151522</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7523630" y="8476130"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>4</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>156883</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>492376</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>79804</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8628530" y="8213912"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>12</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>522195</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>51547</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>857688</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>108939</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8130989" y="8624047"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>13</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>652183</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>13447</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>124823</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>70839</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8260977" y="9347947"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>8</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>423583</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>165847</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>759076</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>32739</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8895230" y="9500347"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>9</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>968189</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>138953</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1303682</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>5845</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9439836" y="9092453"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>10</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>784413</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1119906</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>147039</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9256060" y="8471647"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>11</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1284195</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>6724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1619688</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>64116</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9755842" y="8007724"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>14</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1156448</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1491941</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>171692</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9628095" y="7353300"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>15</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -5157,6 +5969,751 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>31749</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>98985</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="58" name="Picture 57"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect l="18111" r="7694"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3651249" y="5990167"/>
+          <a:ext cx="7115736" cy="3971429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>37371</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>13128</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>372864</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>70520</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4270704" y="8098795"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>18</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>454354</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>123194</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>176013</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>180586</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="60" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4687687" y="7637361"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>17</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>126271</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>91444</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>461764</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>148836</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4359604" y="8748611"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>19</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>529167</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>864660</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>89142</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="62" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7217834" y="8498417"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>22</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>589493</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>89142</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="63" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6942667" y="7164917"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>21</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>385233</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>110067</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>167459</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="64" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6438900" y="7624234"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>26</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>548216</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>188383</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>248709</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>55275</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6601883" y="8274050"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>25</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2116</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>337609</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>38342</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6055783" y="8638117"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>24</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>112183</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>48684</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>447676</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>106076</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4959350" y="8896351"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>20</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>105833</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>39159</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>163225</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="68" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5323416" y="7810500"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>28</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>586315</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>35983</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>149225</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>93375</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5433482" y="8502650"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>29</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>198967</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>71967</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>100543</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>129359</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5818717" y="7395634"/>
+          <a:ext cx="335493" cy="247892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>27</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5203,7 +6760,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5238,7 +6795,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5450,7 +7007,7 @@
   <dimension ref="A1:U55"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="S52" sqref="S45:U52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6891,7 +8448,7 @@
   <dimension ref="A1:U55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Corrected misalignment between generator and .ini file
as per [this comment](https://github.com/robotology/icub-models-generator/pull/248#issuecomment-1721403964) the pictures representing the left and right foot skin patches were not correctly reproducing the actual mounting and .ini file. fixed aligning the depicted positions to the actual ones.
</commit_message>
<xml_diff>
--- a/app/skinGui/iniGenerators/left_foot_ini_generator.xlsx
+++ b/app/skinGui/iniGenerators/left_foot_ini_generator.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\icub-main\app\skinGui\iniGenerators\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SDussoni\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12570" yWindow="-270" windowWidth="12600" windowHeight="12975" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38670" windowHeight="11505"/>
   </bookViews>
   <sheets>
     <sheet name="top" sheetId="1" r:id="rId1"/>
@@ -2127,7 +2127,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>0</a:t>
+            <a:t>10</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2186,7 +2186,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>1</a:t>
+            <a:t>11</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2245,7 +2245,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>2</a:t>
+            <a:t>14</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2304,7 +2304,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>3</a:t>
+            <a:t>15</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2363,7 +2363,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>4</a:t>
+            <a:t>0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2481,7 +2481,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>13</a:t>
+            <a:t>1</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2540,7 +2540,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>8</a:t>
+            <a:t>2</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2599,7 +2599,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>9</a:t>
+            <a:t>3</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2658,7 +2658,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>10</a:t>
+            <a:t>4</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2717,7 +2717,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>11</a:t>
+            <a:t>13</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2776,7 +2776,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>14</a:t>
+            <a:t>8</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2835,7 +2835,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>15</a:t>
+            <a:t>9</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -7006,8 +7006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S52" sqref="S45:U52"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8447,7 +8447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Corrected misalignment between generator and .ini file (#912)
</commit_message>
<xml_diff>
--- a/app/skinGui/iniGenerators/left_foot_ini_generator.xlsx
+++ b/app/skinGui/iniGenerators/left_foot_ini_generator.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\icub-main\app\skinGui\iniGenerators\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SDussoni\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12570" yWindow="-270" windowWidth="12600" windowHeight="12975" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38670" windowHeight="11505"/>
   </bookViews>
   <sheets>
     <sheet name="top" sheetId="1" r:id="rId1"/>
@@ -2127,7 +2127,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>0</a:t>
+            <a:t>10</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2186,7 +2186,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>1</a:t>
+            <a:t>11</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2245,7 +2245,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>2</a:t>
+            <a:t>14</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2304,7 +2304,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>3</a:t>
+            <a:t>15</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2363,7 +2363,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>4</a:t>
+            <a:t>0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2481,7 +2481,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>13</a:t>
+            <a:t>1</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2540,7 +2540,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>8</a:t>
+            <a:t>2</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2599,7 +2599,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>9</a:t>
+            <a:t>3</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2658,7 +2658,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>10</a:t>
+            <a:t>4</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2717,7 +2717,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>11</a:t>
+            <a:t>13</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2776,7 +2776,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>14</a:t>
+            <a:t>8</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2835,7 +2835,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>15</a:t>
+            <a:t>9</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -7006,8 +7006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S52" sqref="S45:U52"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8447,7 +8447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>

</xml_diff>